<commit_message>
update test cases, plan
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="103">
   <si>
     <t>Группа проверок/Модуль</t>
   </si>
@@ -3380,6 +3380,60 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3389,12 +3443,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3405,54 +3453,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3737,8 +3737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3750,13 +3750,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -3764,9 +3764,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="32" t="s">
         <v>32</v>
       </c>
@@ -3786,7 +3786,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="60" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -3800,7 +3800,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -3812,7 +3812,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
@@ -3824,7 +3824,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3836,7 +3836,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="44"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="16" t="s">
         <v>71</v>
       </c>
@@ -3848,7 +3848,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="60" t="s">
         <v>79</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -3862,7 +3862,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3874,7 +3874,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -3886,7 +3886,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="44"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="31" t="s">
         <v>28</v>
       </c>
@@ -3912,7 +3912,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="60" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -3926,7 +3926,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
@@ -3938,7 +3938,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
@@ -3950,7 +3950,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3962,7 +3962,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
@@ -3986,7 +3986,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="44"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
       </c>
@@ -3998,7 +3998,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="60" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -4012,7 +4012,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="43"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
@@ -4024,7 +4024,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
@@ -4036,7 +4036,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="44"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="16" t="s">
         <v>11</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="55" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -4062,7 +4062,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
@@ -4074,7 +4074,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="3" t="s">
         <v>42</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="51"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="23" t="s">
         <v>21</v>
       </c>
@@ -4098,7 +4098,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="53" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -4112,7 +4112,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="53"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
@@ -4136,7 +4136,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="1" t="s">
         <v>46</v>
       </c>
@@ -4148,7 +4148,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="1" t="s">
         <v>47</v>
       </c>
@@ -4160,7 +4160,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="44"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="16" t="s">
         <v>48</v>
       </c>
@@ -4172,17 +4172,21 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="55" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
+      <c r="C35" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="50"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
@@ -4194,15 +4198,19 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="50"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="15"/>
+      <c r="C37" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="3" t="s">
         <v>49</v>
       </c>
@@ -4214,7 +4222,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="50"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="3" t="s">
         <v>20</v>
       </c>
@@ -4226,7 +4234,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="51"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="23" t="s">
         <v>21</v>
       </c>
@@ -4238,7 +4246,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="43" t="s">
         <v>83</v>
       </c>
       <c r="B41" s="12" t="s">
@@ -4252,7 +4260,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="55"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
@@ -4264,7 +4272,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
@@ -4276,7 +4284,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="55"/>
+      <c r="A44" s="54"/>
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
@@ -4288,7 +4296,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="55"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="1" t="s">
         <v>12</v>
       </c>
@@ -4300,7 +4308,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="56"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="16" t="s">
         <v>54</v>
       </c>
@@ -4312,7 +4320,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="55" t="s">
         <v>84</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -4326,7 +4334,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="3" t="s">
         <v>75</v>
       </c>
@@ -4338,7 +4346,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="50"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="3" t="s">
         <v>56</v>
       </c>
@@ -4350,7 +4358,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="51"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="23" t="s">
         <v>57</v>
       </c>
@@ -4362,7 +4370,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="54" t="s">
+      <c r="A51" s="43" t="s">
         <v>98</v>
       </c>
       <c r="B51" s="12" t="s">
@@ -4376,7 +4384,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="58"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="1" t="s">
         <v>14</v>
       </c>
@@ -4388,7 +4396,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="59"/>
+      <c r="A53" s="45"/>
       <c r="B53" s="16" t="s">
         <v>99</v>
       </c>
@@ -4400,7 +4408,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="60" t="s">
+      <c r="A54" s="46" t="s">
         <v>85</v>
       </c>
       <c r="B54" s="20" t="s">
@@ -4414,7 +4422,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="23" t="s">
         <v>58</v>
       </c>
@@ -4426,7 +4434,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="48" t="s">
         <v>86</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -4440,7 +4448,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="53"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="1" t="s">
         <v>97</v>
       </c>
@@ -4452,7 +4460,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="53"/>
+      <c r="A58" s="49"/>
       <c r="B58" s="1" t="s">
         <v>60</v>
       </c>
@@ -4464,7 +4472,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="53"/>
+      <c r="A59" s="49"/>
       <c r="B59" s="1" t="s">
         <v>15</v>
       </c>
@@ -4476,7 +4484,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="63"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="16" t="s">
         <v>61</v>
       </c>
@@ -4488,7 +4496,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="62" t="s">
+      <c r="A61" s="48" t="s">
         <v>96</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -4502,7 +4510,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="53"/>
+      <c r="A62" s="49"/>
       <c r="B62" s="1" t="s">
         <v>62</v>
       </c>
@@ -4514,7 +4522,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="53"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="1" t="s">
         <v>63</v>
       </c>
@@ -4526,7 +4534,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="53"/>
+      <c r="A64" s="49"/>
       <c r="B64" s="1" t="s">
         <v>64</v>
       </c>
@@ -4538,7 +4546,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="53"/>
+      <c r="A65" s="49"/>
       <c r="B65" s="1" t="s">
         <v>65</v>
       </c>
@@ -4550,7 +4558,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="64"/>
+      <c r="A66" s="51"/>
       <c r="B66" s="9" t="s">
         <v>16</v>
       </c>
@@ -4562,7 +4570,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="52" t="s">
+      <c r="A67" s="53" t="s">
         <v>93</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -4576,15 +4584,19 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="55"/>
+      <c r="A68" s="54"/>
       <c r="B68" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="39"/>
+      <c r="C68" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="63"/>
+      <c r="A69" s="50"/>
       <c r="B69" s="16" t="s">
         <v>94</v>
       </c>
@@ -4596,7 +4608,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="62" t="s">
+      <c r="A70" s="48" t="s">
         <v>87</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -4610,7 +4622,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="44"/>
+      <c r="A71" s="52"/>
       <c r="B71" s="16" t="s">
         <v>18</v>
       </c>
@@ -4622,7 +4634,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="57" t="s">
+      <c r="A72" s="40" t="s">
         <v>88</v>
       </c>
       <c r="B72" s="12" t="s">
@@ -4631,10 +4643,12 @@
       <c r="C72" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="14"/>
+      <c r="D72" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="50"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="3" t="s">
         <v>23</v>
       </c>
@@ -4646,7 +4660,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="50"/>
+      <c r="A74" s="41"/>
       <c r="B74" s="3" t="s">
         <v>24</v>
       </c>
@@ -4658,7 +4672,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="50"/>
+      <c r="A75" s="41"/>
       <c r="B75" s="3" t="s">
         <v>22</v>
       </c>
@@ -4670,7 +4684,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="50"/>
+      <c r="A76" s="41"/>
       <c r="B76" s="3" t="s">
         <v>66</v>
       </c>
@@ -4682,7 +4696,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="51"/>
+      <c r="A77" s="42"/>
       <c r="B77" s="23" t="s">
         <v>67</v>
       </c>
@@ -4694,7 +4708,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="57" t="s">
+      <c r="A78" s="40" t="s">
         <v>89</v>
       </c>
       <c r="B78" s="20" t="s">
@@ -4708,7 +4722,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="50"/>
+      <c r="A79" s="41"/>
       <c r="B79" s="3" t="s">
         <v>26</v>
       </c>
@@ -4720,7 +4734,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="50"/>
+      <c r="A80" s="41"/>
       <c r="B80" s="3" t="s">
         <v>25</v>
       </c>
@@ -4732,7 +4746,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="50"/>
+      <c r="A81" s="41"/>
       <c r="B81" s="3" t="s">
         <v>68</v>
       </c>
@@ -4744,7 +4758,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="51"/>
+      <c r="A82" s="42"/>
       <c r="B82" s="37" t="s">
         <v>27</v>
       </c>
@@ -4803,6 +4817,18 @@
     <row r="137" ht="173.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A35:A40"/>
     <mergeCell ref="A72:A77"/>
     <mergeCell ref="A78:A82"/>
     <mergeCell ref="A51:A53"/>
@@ -4811,18 +4837,6 @@
     <mergeCell ref="A61:A66"/>
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>